<commit_message>
[woo] first_reward 테이블의 초기 지급 id spell -> source
</commit_message>
<xml_diff>
--- a/GameData/Excel/first_reward.xlsx
+++ b/GameData/Excel/first_reward.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\Go.D.Taekwon\GameData\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB27C29-B0F3-42CF-AFAC-E11C47437F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB3DB34-8302-4218-B942-753A9220C33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="3300" windowWidth="21600" windowHeight="11430" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
+    <workbookView xWindow="15144" yWindow="11712" windowWidth="20328" windowHeight="12720" xr2:uid="{31F9D538-CB36-4F6C-AC31-CCD9A4836B67}"/>
   </bookViews>
   <sheets>
     <sheet name="first_reward" sheetId="1" r:id="rId1"/>
@@ -53,14 +53,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>spell_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>초기 스펠 셋팅</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -77,6 +69,14 @@
   </si>
   <si>
     <t>first_reward_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>source_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지급할 근원 ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -510,61 +510,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D9A91B-D08A-4539-AB73-212820098BCC}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="2" width="12" style="3" customWidth="1"/>
     <col min="3" max="4" width="25" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.75" style="3"/>
+    <col min="5" max="16384" width="8.69921875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="5" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1000001</v>
       </c>
@@ -572,13 +572,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>10001</v>
+        <v>1001</v>
       </c>
       <c r="D4" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1000001</v>
       </c>
@@ -586,89 +586,83 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>10002</v>
+        <v>1003</v>
       </c>
       <c r="D5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>